<commit_message>
Finished data cleaning code, still need to export results to csv
</commit_message>
<xml_diff>
--- a/Counties List.xlsx
+++ b/Counties List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/courtneymacdonald/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/courtneymacdonald/Desktop/Homelessness-Weather/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61379AE0-087E-974B-8FAF-16CB9C1BDDC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A504D08D-481A-9A4E-807C-43E6896AA3B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1540" windowWidth="14700" windowHeight="16460" xr2:uid="{43206EC6-9CFC-0241-983F-1EA987D2FBE7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>City</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Los Angeles County</t>
   </si>
   <si>
-    <t>San Fransisco</t>
-  </si>
-  <si>
-    <t>San Fransisco County</t>
-  </si>
-  <si>
     <t>Las Vegas</t>
   </si>
   <si>
@@ -160,6 +154,69 @@
   </si>
   <si>
     <t>Hennepin County</t>
+  </si>
+  <si>
+    <t>Bernalillo_County</t>
+  </si>
+  <si>
+    <t>Clark_County</t>
+  </si>
+  <si>
+    <t>Cook_County</t>
+  </si>
+  <si>
+    <t>Dade_County</t>
+  </si>
+  <si>
+    <t>Dallas_County</t>
+  </si>
+  <si>
+    <t>Davidson_County</t>
+  </si>
+  <si>
+    <t>Denver_County</t>
+  </si>
+  <si>
+    <t>Fulton_County</t>
+  </si>
+  <si>
+    <t>Hennepin_County</t>
+  </si>
+  <si>
+    <t>Jackson_County</t>
+  </si>
+  <si>
+    <t>King_County</t>
+  </si>
+  <si>
+    <t>Los_Angeles_County</t>
+  </si>
+  <si>
+    <t>Maricopa_County</t>
+  </si>
+  <si>
+    <t>Marion_County</t>
+  </si>
+  <si>
+    <t>New_York_County</t>
+  </si>
+  <si>
+    <t>Philadelphia_County</t>
+  </si>
+  <si>
+    <t>Suffolk_County</t>
+  </si>
+  <si>
+    <t>Wayne_County</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>San Francisco County</t>
+  </si>
+  <si>
+    <t>San_Francisco_County</t>
   </si>
 </sst>
 </file>
@@ -521,19 +578,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDD903D-308E-624B-A320-924E61407507}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,18 +600,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -560,208 +622,268 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D21">
+    <sortCondition ref="B2:B21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>